<commit_message>
add diff command in XLS
</commit_message>
<xml_diff>
--- a/git_learning_summary.xlsx
+++ b/git_learning_summary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>git 学习笔记</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,6 +63,58 @@
   </si>
   <si>
     <t>git checkout -- &lt;file&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7 查看更改记录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P.S 几个命令间的关系</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. 恢复到上一个记录点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get reset HEAD~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用命令前</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P.S: reset命令各个参数间的差异</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用命令后</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P.S: 文本文档尽量用UTF-8来保存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8. git diff 比较两个文档差异</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无参数比较当前working目录下和暂存区里的数据差异</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前和最新的快照对比</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git diff HEAD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -390,6 +442,523 @@
         <a:xfrm>
           <a:off x="0" y="14782800"/>
           <a:ext cx="5905500" cy="3505200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="18859500"/>
+          <a:ext cx="5038725" cy="2247900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="21602700"/>
+          <a:ext cx="5743575" cy="3743325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="26231850"/>
+          <a:ext cx="3990975" cy="3648075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>178</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>203</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="30518100"/>
+          <a:ext cx="6191250" cy="4438650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4114800" y="26231850"/>
+          <a:ext cx="4067175" cy="3590925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>204</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>218</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="34975800"/>
+          <a:ext cx="6543675" cy="2533650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>222</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>236</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="38061900"/>
+          <a:ext cx="5276850" cy="2400300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>242</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>258</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="41490900"/>
+          <a:ext cx="4714875" cy="2895600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>260</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>276</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="44577000"/>
+          <a:ext cx="6038850" cy="2828925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>281</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>293</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="48177450"/>
+          <a:ext cx="3848100" cy="2152650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>295</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>320</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="50577750"/>
+          <a:ext cx="5829300" cy="4419600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -694,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:H279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
+      <selection activeCell="A296" sqref="A296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -756,6 +1325,65 @@
     <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
+        <v>12</v>
+      </c>
+      <c r="C110" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8">
+      <c r="A151" t="s">
+        <v>15</v>
+      </c>
+      <c r="D151" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8">
+      <c r="B153" t="s">
+        <v>17</v>
+      </c>
+      <c r="H153" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1">
+      <c r="A240" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="241" spans="2:2">
+      <c r="B241" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1">
+      <c r="A278" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1">
+      <c r="A279" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
learning summary on 2019.2.17 morning
</commit_message>
<xml_diff>
--- a/git_learning_summary.xlsx
+++ b/git_learning_summary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>git 学习笔记</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -115,6 +115,33 @@
   </si>
   <si>
     <t>git diff HEAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9. git clone 用来copy其他人的项目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10. git commit的小技巧</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>远程 git 库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/</t>
+  </si>
+  <si>
+    <t>建立一个远程库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将本地库的内容推送到远程库上</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git clone 的一些注意点。。。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -959,6 +986,429 @@
         <a:xfrm>
           <a:off x="0" y="50577750"/>
           <a:ext cx="5829300" cy="4419600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>324</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>369</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="55549800"/>
+          <a:ext cx="11096625" cy="7829550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>373</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>393</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="63950850"/>
+          <a:ext cx="12573000" cy="3514725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>393</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>552451</xdr:colOff>
+      <xdr:row>415</xdr:row>
+      <xdr:rowOff>93199</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1" y="67522725"/>
+          <a:ext cx="12896850" cy="3722224"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>416</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>631841</xdr:colOff>
+      <xdr:row>426</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="71323201"/>
+          <a:ext cx="6118241" cy="1809750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>433</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>468</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="74237850"/>
+          <a:ext cx="7486650" cy="6096000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>471</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>522414</xdr:colOff>
+      <xdr:row>506</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="80752950"/>
+          <a:ext cx="8066214" cy="6010275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>506</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>527</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="86839425"/>
+          <a:ext cx="13144500" cy="3619500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>528</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>538</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1030" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="90525600"/>
+          <a:ext cx="13049250" cy="1714500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>540</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>550</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1031" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="92583000"/>
+          <a:ext cx="12582525" cy="1828800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1263,10 +1713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H279"/>
+  <dimension ref="A1:H540"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
-      <selection activeCell="A296" sqref="A296"/>
+    <sheetView tabSelected="1" topLeftCell="A511" workbookViewId="0">
+      <selection activeCell="A541" sqref="A541"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1384,6 +1834,41 @@
     <row r="279" spans="1:1">
       <c r="A279" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1">
+      <c r="A324" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1">
+      <c r="A373" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1">
+      <c r="A429" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1">
+      <c r="A431" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1">
+      <c r="A433" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1">
+      <c r="A471" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="540" spans="1:1">
+      <c r="A540" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>